<commit_message>
debut du scenario liste de chaine
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
@@ -653,6 +653,28 @@
           <t>pass</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>frbfnpkfsxoupxa@gmail.com</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>oiypuLOKPS5</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Première phase de clean code
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -435,10 +435,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -574,103 +574,15 @@
     <row r="5">
       <c r="C5" t="inlineStr">
         <is>
-          <t>lhmijojyjrojduc@gmail.com</t>
+          <t>bmkbihhxjvucvxk@gmail.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>jzzbjELMQY5</t>
+          <t>rvjycHYANC5</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>jkscrhxnlkgeonw@gmail.com</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>pckegEKNVK5</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>acocbuuomnfvzjp@gmail.com</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>aqvzlVZHIU5</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>mnzgvbnfzffydsw@gmail.com</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>wivcsCGWRB5</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>frbfnpkfsxoupxa@gmail.com</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>oiypuLOKPS5</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
         <is>
           <t>pass</t>
         </is>

</xml_diff>

<commit_message>
fin du 3eme scénario
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -435,10 +435,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -574,15 +574,81 @@
     <row r="5">
       <c r="C5" t="inlineStr">
         <is>
-          <t>bmkbihhxjvucvxk@gmail.com</t>
+          <t>xeumeaauflczvbx@gmail.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>rvjycHYANC5</t>
+          <t>mluklKTDCO5</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>vhnjnquirwqrosv@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>yicovWOHEI5</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ubizvtrlheyavla@gmail.com</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>ipnyyYETFZ5</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>lddawxqfztqllxu@gmail.com</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>yqdesHMCPL5</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>pass</t>
         </is>

</xml_diff>

<commit_message>
Après la mise a jour de script shell, 3 commandes en one shot
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -1,114 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdi.bileh17/Documents/Selenium/Projet_test_v0/TestData/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F440F39C-056F-A04D-BADB-7D3E36873DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
-  <si>
-    <t>prenom</t>
-  </si>
-  <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>mdp</t>
-  </si>
-  <si>
-    <t>exp</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>abdi.bilehm6@gmail.com</t>
-  </si>
-  <si>
-    <t>bonjourA1</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>abdi.bilehm@gmail.com</t>
-  </si>
-  <si>
-    <t>blablablaP0</t>
-  </si>
-  <si>
-    <t>fail</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>abdi.bilehm99@gmail.com</t>
-  </si>
-  <si>
-    <t>helloA11</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="12"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -128,23 +55,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -444,99 +430,185 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>prenom</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Nom</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>mdp</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>exp</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>abdi.bilehm6@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>bonjourA1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>FAIL</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>abdi.bilehm@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>blablablaP0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>fail</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>abdi.bilehm99@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>helloA11</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>qspuolucvvmjsjs@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>iqrgjKLACP5</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>pjiifucrlneizxf@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ldemoGOEKB5</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
premier test avec allure reporting
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
@@ -503,7 +503,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -587,6 +587,11 @@
           <t>pass</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="C6" t="inlineStr">
@@ -600,6 +605,72 @@
         </is>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>kuqnabgrrdhrdpd@gmail.com</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>vhtvsMFBFZ5</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>uuvqmhzknkmjnpc@gmail.com</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>vytszXNSCT5</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ycwlrrnwcgpzsgf@gmail.com</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>fejnwTVDEH5</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>pass</t>
         </is>

</xml_diff>

<commit_message>
Maj de fichier bash avec la génération de rapport allure + sleep
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -675,6 +675,11 @@
           <t>pass</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
deuxieme jet de nettoyage de code version 0
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdi.bileh17/Documents/Selenium/Projet_test_v0/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196916C7-13E3-6E49-A4F7-B184E17165CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A1E124-5051-C748-890C-6EA767622FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -448,7 +448,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="B5" sqref="B5:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update obPage file using action_OnElem class-After fixing action_OnElem instance error in ObPage.py
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -1,114 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdi.bileh17/Documents/Selenium/Projet_test_v0/TestData/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A1E124-5051-C748-890C-6EA767622FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
-  <si>
-    <t>prenom</t>
-  </si>
-  <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>mdp</t>
-  </si>
-  <si>
-    <t>exp</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>abdi.bilehm6@gmail.com</t>
-  </si>
-  <si>
-    <t>bonjourA1</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>abdi.bilehm@gmail.com</t>
-  </si>
-  <si>
-    <t>blablablaP0</t>
-  </si>
-  <si>
-    <t>fail</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>abdi.bilehm99@gmail.com</t>
-  </si>
-  <si>
-    <t>helloA11</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="12"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -128,23 +55,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -444,99 +430,168 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>prenom</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Nom</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>mdp</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>exp</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>abdi.bilehm6@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>bonjourA1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>abdi.bilehm@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>blablablaP0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>fail</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>abdi.bilehm99@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>helloA11</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>iigapzgiadqkjty@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>hcmijHFPVO5</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update obPage file using action_OnElem class-After fixing action_OnElem instance error in homePage.py
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:G10"/>
@@ -587,6 +587,50 @@
           <t>pass</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>epljxtvbgwbcxyl@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>iltovYZDUX5</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ljrhsjgymlygiyx@gmail.com</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>rielwWEGCW5</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
after managing some files and fixed several errors
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -438,7 +438,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:G10"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -574,12 +574,12 @@
     <row r="5">
       <c r="C5" t="inlineStr">
         <is>
-          <t>iigapzgiadqkjty@gmail.com</t>
+          <t>xcgbjaeitgbvzmt@gmail.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>hcmijHFPVO5</t>
+          <t>sjlrlLKJSB5</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -596,12 +596,12 @@
     <row r="6">
       <c r="C6" t="inlineStr">
         <is>
-          <t>epljxtvbgwbcxyl@gmail.com</t>
+          <t>xiytnjkplizixwd@gmail.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>iltovYZDUX5</t>
+          <t>yhoqqXQNPK5</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -618,12 +618,12 @@
     <row r="7">
       <c r="C7" t="inlineStr">
         <is>
-          <t>ljrhsjgymlygiyx@gmail.com</t>
+          <t>wvadvqtseuzaftr@gmail.com</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>rielwWEGCW5</t>
+          <t>glcbqYPPYZ5</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">

</xml_diff>

<commit_message>
after fixing some problem with liste elements (chaine))
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
@@ -435,13 +435,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col width="29.6640625" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -574,12 +577,12 @@
     <row r="5">
       <c r="C5" t="inlineStr">
         <is>
-          <t>xcgbjaeitgbvzmt@gmail.com</t>
+          <t>gkqsvvoniujdguz@gmail.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>sjlrlLKJSB5</t>
+          <t>locnaIKOUE5</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -596,37 +599,15 @@
     <row r="6">
       <c r="C6" t="inlineStr">
         <is>
-          <t>xiytnjkplizixwd@gmail.com</t>
+          <t>covxqsvvpyvvwlx@gmail.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>yhoqqXQNPK5</t>
+          <t>wrbzmVYMMN5</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>wvadvqtseuzaftr@gmail.com</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>glcbqYPPYZ5</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
         <is>
           <t>pass</t>
         </is>

</xml_diff>

<commit_message>
un test pour voir si le git ignore fonctionne correctement
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
@@ -612,6 +612,33 @@
           <t>pass</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>sarzigptgnrrjrf@gmail.com</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>wcsjcRVJTP5</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
refacto common_action avec facto self.wait + ignore tous les fichier pycache
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
@@ -435,10 +435,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -577,66 +577,17 @@
     <row r="5">
       <c r="C5" t="inlineStr">
         <is>
-          <t>gkqsvvoniujdguz@gmail.com</t>
+          <t>eogaxjynuzvkhno@gmail.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>locnaIKOUE5</t>
+          <t>qfgqfXQUGL5</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>pass</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>covxqsvvpyvvwlx@gmail.com</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>wrbzmVYMMN5</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>sarzigptgnrrjrf@gmail.com</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>wcsjcRVJTP5</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>PASS</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ignore tous les dossiers pycache
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
@@ -590,6 +590,28 @@
           <t>pass</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>xfsimmvonglnkvk@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>opqfmLGASI5</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Suppression des nouveaux ID dans le fichier excel
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -1,41 +1,114 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdi.bileh17/Documents/Selenium/Projet_test_v0/TestData/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0510C0A-5D32-F649-A07E-72DCB8DEA113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+  <si>
+    <t>prenom</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>mdp</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>abdi.bilehm6@gmail.com</t>
+  </si>
+  <si>
+    <t>bonjourA1</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>abdi.bilehm@gmail.com</t>
+  </si>
+  <si>
+    <t>blablablaP0</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>abdi.bilehm99@gmail.com</t>
+  </si>
+  <si>
+    <t>helloA11</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="10"/>
-      <sz val="12"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -55,82 +128,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -430,193 +444,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col width="29.6640625" customWidth="1" min="3" max="3"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>prenom</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Nom</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>mdp</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>exp</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>abdi.bilehm6@gmail.com</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>bonjourA1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>abdi.bilehm@gmail.com</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>blablablaP0</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>fail</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>abdi.bilehm99@gmail.com</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>helloA11</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>eogaxjynuzvkhno@gmail.com</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>qfgqfXQUGL5</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>xfsimmvonglnkvk@gmail.com</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>opqfmLGASI5</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
review de la recup de donnee d'un element, fichier comme_action.py et HomePage.py
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -1,114 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdi.bileh17/Documents/Selenium/Projet_test_v0/TestData/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0510C0A-5D32-F649-A07E-72DCB8DEA113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
-  <si>
-    <t>prenom</t>
-  </si>
-  <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>mdp</t>
-  </si>
-  <si>
-    <t>exp</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>abdi.bilehm6@gmail.com</t>
-  </si>
-  <si>
-    <t>bonjourA1</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>abdi.bilehm@gmail.com</t>
-  </si>
-  <si>
-    <t>blablablaP0</t>
-  </si>
-  <si>
-    <t>fail</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>abdi.bilehm99@gmail.com</t>
-  </si>
-  <si>
-    <t>helloA11</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="12"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -128,23 +55,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -444,102 +430,171 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col width="29.6640625" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>prenom</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Nom</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>mdp</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>exp</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>abdi.bilehm6@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>bonjourA1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>abdi.bilehm@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>blablablaP0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>fail</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>abdi.bilehm99@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>helloA11</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>iwdccjxqklaosng@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>fjsywSKFJK5</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout de colonnes fichier excel
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -1,41 +1,123 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdi.bileh17/Documents/Selenium/Projet_test_v0/TestData/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84F6C1D-7D56-3947-9414-7CD4702DEB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+  <si>
+    <t>prenom</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>mdp</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>abdi.bilehm6@gmail.com</t>
+  </si>
+  <si>
+    <t>bonjourA1</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>abdi.bilehm@gmail.com</t>
+  </si>
+  <si>
+    <t>blablablaP0</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>abdi.bilehm99@gmail.com</t>
+  </si>
+  <si>
+    <t>helloA11</t>
+  </si>
+  <si>
+    <t>date_naissance</t>
+  </si>
+  <si>
+    <t>date_créa</t>
+  </si>
+  <si>
+    <t>dernière date_co</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="10"/>
-      <sz val="12"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -55,82 +137,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -430,171 +453,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col width="29.6640625" customWidth="1" min="3" max="3"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>prenom</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Nom</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>mdp</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>exp</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>abdi.bilehm6@gmail.com</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>bonjourA1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>abdi.bilehm@gmail.com</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>blablablaP0</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>fail</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>abdi.bilehm99@gmail.com</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>helloA11</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>iwdccjxqklaosng@gmail.com</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>fjsywSKFJK5</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout action common checker jusqu'a l'invisibilité de l'element
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -1,123 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdi.bileh17/Documents/Selenium/Projet_test_v0/TestData/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84F6C1D-7D56-3947-9414-7CD4702DEB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
-  <si>
-    <t>prenom</t>
-  </si>
-  <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>mdp</t>
-  </si>
-  <si>
-    <t>exp</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>abdi.bilehm6@gmail.com</t>
-  </si>
-  <si>
-    <t>bonjourA1</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>abdi.bilehm@gmail.com</t>
-  </si>
-  <si>
-    <t>blablablaP0</t>
-  </si>
-  <si>
-    <t>fail</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>abdi.bilehm99@gmail.com</t>
-  </si>
-  <si>
-    <t>helloA11</t>
-  </si>
-  <si>
-    <t>date_naissance</t>
-  </si>
-  <si>
-    <t>date_créa</t>
-  </si>
-  <si>
-    <t>dernière date_co</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="12"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -137,23 +55,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -453,111 +430,169 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col width="29.6640625" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>prenom</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Nom</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>date_naissance</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>mdp</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>exp</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>date_créa</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>dernière date_co</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>abdi.bilehm6@gmail.com</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>bonjourA1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>abdi.bilehm@gmail.com</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>blablablaP0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>fail</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>abdi.bilehm99@gmail.com</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>helloA11</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Version Beta - ajout des assets au 3 scénario + ajouts des objets dans le locators et action
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -1,41 +1,136 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdi.bileh17/Documents/Selenium/Projet_test_v0/TestData/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF6D448-5248-194B-B614-CAD81B123CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="DonneesUser" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+  <si>
+    <t>prenom</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>date_naissance</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>mdp</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>date_créa</t>
+  </si>
+  <si>
+    <t>dernière date_co</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>abdi.bilehm6@gmail.com</t>
+  </si>
+  <si>
+    <t>bonjourA1</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>abdi.bilehm@gmail.com</t>
+  </si>
+  <si>
+    <t>blablablaP0</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>abdi.bilehm99@gmail.com</t>
+  </si>
+  <si>
+    <t>helloA11</t>
+  </si>
+  <si>
+    <t>nom</t>
+  </si>
+  <si>
+    <t>dateNaissance</t>
+  </si>
+  <si>
+    <t>genre</t>
+  </si>
+  <si>
+    <t>progFavoris</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="10"/>
-      <sz val="12"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -55,82 +150,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -430,170 +466,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col width="29.6640625" customWidth="1" min="4" max="4"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>prenom</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Nom</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>date_naissance</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>mdp</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>exp</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>date_créa</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>dernière date_co</t>
-        </is>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>abdi.bilehm6@gmail.com</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>bonjourA1</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="D3" s="1" t="inlineStr">
-        <is>
-          <t>abdi.bilehm@gmail.com</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>blablablaP0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>fail</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>abdi.bilehm99@gmail.com</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>helloA11</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D647FC-7DE5-D441-AE25-6482314FD817}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
qlq modif + maj fichier ignore
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -678,6 +678,50 @@
         </is>
       </c>
       <c r="F8" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>23/07/1992</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>xkknnasnpqpxdzj@gmail.com</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>pmpbuTRSZW5</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>19/12/1990</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>epmxnqagoyunrzs@gmail.com</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>bjnfdMIOHT5</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
         <is>
           <t>pass</t>
         </is>

</xml_diff>

<commit_message>
ajout de log dans le test connexion
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -436,10 +436,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -549,12 +549,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>fail</t>
+          <t>pass</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>PASS</t>
+          <t>FAIL</t>
         </is>
       </c>
     </row>
@@ -722,6 +722,116 @@
         </is>
       </c>
       <c r="F10" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>12/10/1978</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ujpshrhgrcukjbb@gmail.com</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>kseecZQOLJ5</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>30/12/1989</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>ajcsxgxcjbnrypl@gmail.com</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>diwmcWKCOB5</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>04/09/1977</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>euygnnbmxacyhco@gmail.com</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>sstglAVTKQ5</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>14/12/1981</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>erobvegrhbxuncq@gmail.com</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>alqmtSAKWZ5</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>23/11/2004</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>orkmjqjqnosdhqi@gmail.com</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>sgshzWELWB5</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
         <is>
           <t>pass</t>
         </is>

</xml_diff>

<commit_message>
maj de fichier excel
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -832,6 +832,50 @@
         </is>
       </c>
       <c r="F15" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>14/08/1997</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>xaprkkcwssjkbsl@gmail.com</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>neddhSAIKM5</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>17/01/1984</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>bjveamxemxbginv@gmail.com</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>mvmugZZFRW5</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
         <is>
           <t>pass</t>
         </is>

</xml_diff>

<commit_message>
maj conftest + maj Run.sh pour effetcuer de tests sans rapport allure
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -436,10 +436,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -549,12 +549,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -876,6 +876,94 @@
         </is>
       </c>
       <c r="F17" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>09/01/2001</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>opqsleciiggdhik@gmail.com</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>wdmujKSMZF5</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>17/07/1992</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>bbchdfmnfrcpkgm@gmail.com</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>dsmtzHUSSJ5</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>28/09/1974</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>oqvbovkticuqkqb@gmail.com</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>tepfsZSOFA5</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>24/06/1992</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>ccjatqnecgvwuey@gmail.com</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>xdtpcXQAEI5</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
         <is>
           <t>pass</t>
         </is>

</xml_diff>

<commit_message>
reorganisation des actions dans les scripts POM
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
@@ -964,6 +964,28 @@
         </is>
       </c>
       <c r="F21" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>24/07/2005</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>nbrnneputiqtwys@gmail.com</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>goevbULWSS5</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
         <is>
           <t>pass</t>
         </is>

</xml_diff>